<commit_message>
la concha de la lora entrega de formacion de la puta madre.png
</commit_message>
<xml_diff>
--- a/ProyectoMaterias/Formación/Materiales lista precioimport vs precio.xlsx
+++ b/ProyectoMaterias/Formación/Materiales lista precioimport vs precio.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Material</t>
   </si>
@@ -188,12 +188,6 @@
   </si>
   <si>
     <t>Mesa para la cocina (con sillas)</t>
-  </si>
-  <si>
-    <t>2 (6)</t>
-  </si>
-  <si>
-    <t>10 de cada y un escurridor</t>
   </si>
   <si>
     <t>----------------</t>
@@ -218,7 +212,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,12 +227,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -262,6 +250,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -364,49 +363,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -725,7 +747,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,28 +756,28 @@
     <col min="2" max="2" width="39.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>60</v>
+      <c r="E1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -772,7 +794,7 @@
       <c r="E2" s="16">
         <v>985</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="13">
         <f>E2*D2</f>
         <v>6895</v>
       </c>
@@ -791,7 +813,7 @@
       <c r="E3" s="17">
         <v>599</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="14">
         <f>E3*D3</f>
         <v>11980</v>
       </c>
@@ -807,8 +829,13 @@
       <c r="D4" s="3">
         <v>10</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="18">
+        <v>400</v>
+      </c>
+      <c r="F4" s="14">
+        <f t="shared" ref="F4:F13" si="0">E4*D4</f>
+        <v>4000</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -818,9 +845,16 @@
       <c r="C5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1390</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" si="0"/>
+        <v>2780</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -833,8 +867,13 @@
       <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="18">
+        <v>3790</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="0"/>
+        <v>3790</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -844,11 +883,16 @@
       <c r="C7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>14990</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="0"/>
+        <v>29980</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -861,8 +905,13 @@
       <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="18">
+        <v>2815</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="0"/>
+        <v>2815</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -875,8 +924,13 @@
       <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="18">
+        <v>7968</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="0"/>
+        <v>7968</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -886,11 +940,14 @@
       <c r="C10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -903,8 +960,11 @@
       <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -917,8 +977,11 @@
       <c r="D12" s="3">
         <v>7</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -931,15 +994,18 @@
       <c r="D13" s="3">
         <v>3</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -949,7 +1015,7 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -963,7 +1029,7 @@
       <c r="D16" s="3">
         <v>8</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -977,7 +1043,7 @@
       <c r="D17" s="3">
         <v>12</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -991,7 +1057,7 @@
       <c r="D18" s="3">
         <v>1</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1005,7 +1071,7 @@
       <c r="D19" s="3">
         <v>1</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="20"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1019,7 +1085,7 @@
       <c r="D20" s="3">
         <v>2</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1033,7 +1099,7 @@
       <c r="D21" s="3">
         <v>2</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1047,7 +1113,7 @@
       <c r="D22" s="3">
         <v>4</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1061,7 +1127,7 @@
       <c r="D23" s="3">
         <v>3</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
@@ -1075,7 +1141,7 @@
       <c r="D24" s="3">
         <v>3</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1083,17 +1149,17 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="E25" s="21"/>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1105,9 +1171,9 @@
         <v>52</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E27" s="20"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1119,9 +1185,9 @@
         <v>52</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E28" s="20"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1133,9 +1199,9 @@
         <v>52</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E29" s="20"/>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1147,9 +1213,9 @@
         <v>52</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E30" s="20"/>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1158,12 +1224,12 @@
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E31" s="20"/>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1175,9 +1241,9 @@
         <v>52</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E32" s="20"/>
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1186,12 +1252,12 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E33" s="20"/>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1200,12 +1266,12 @@
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E34" s="20"/>
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1219,9 +1285,9 @@
         <v>50</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E35" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="23" t="s">
         <v>4</v>
       </c>
       <c r="F35" s="4"/>
@@ -1237,9 +1303,9 @@
         <v>50</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F36" s="4"/>
@@ -1255,9 +1321,9 @@
         <v>50</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="20" t="s">
         <v>10</v>
       </c>
       <c r="F37" s="4"/>
@@ -1273,9 +1339,9 @@
         <v>50</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="20" t="s">
         <v>10</v>
       </c>
       <c r="F38" s="4"/>
@@ -1291,9 +1357,9 @@
         <v>50</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="23" t="s">
         <v>15</v>
       </c>
       <c r="F39" s="4"/>
@@ -1309,9 +1375,9 @@
         <v>50</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="23" t="s">
         <v>18</v>
       </c>
       <c r="F40" s="4"/>
@@ -1323,8 +1389,15 @@
     <hyperlink ref="E39" r:id="rId3"/>
     <hyperlink ref="E36" r:id="rId4"/>
     <hyperlink ref="E2" r:id="rId5" display="https://articulo.mercadolibre.com.uy/MLU-445279074-escritorio-mesa-de-pc-con-cajon-oficina-mueble-lcm-_JM"/>
+    <hyperlink ref="E5" r:id="rId6" display="https://articulo.mercadolibre.com.uy/MLU-442899266-mueble-cocina-multiuso-armari-living-oficina-2401-_JM"/>
+    <hyperlink ref="E3" r:id="rId7" display="https://articulo.mercadolibre.com.uy/MLU-443808655-silla-fija-eco-de-escritorio-oficina-hogar-apilable-armada-_JM"/>
+    <hyperlink ref="E4" r:id="rId8" display="https://articulo.mercadolibre.com.uy/MLU-452988688-artefacto-tubo-led-doble-36w-120cm-blanco-frio-6500-k-_JM"/>
+    <hyperlink ref="E6" r:id="rId9" display="https://articulo.mercadolibre.com.uy/MLU-444421998-sillon-sofa-3-lugares-minimalista-mesa-y-2-puff--_JM"/>
+    <hyperlink ref="E7" r:id="rId10" display="https://articulo.mercadolibre.com.uy/MLU-444478827-juego-de-mesa-y-sillas-comedor-o-cocina-varios-modelos-gh-_JM"/>
+    <hyperlink ref="E8" r:id="rId11" display="https://articulo.mercadolibre.com.uy/MLU-447144410-microondas-panavox-express-20-digital-el-mejor-respaldo-_JM"/>
+    <hyperlink ref="E9" r:id="rId12" display="https://articulo.mercadolibre.com.uy/MLU-452575969-refrigerador-heladera-electrolux-re31-de-240l-oferta-loi-_JM"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se agregaron inversiones iniciales excel formacion
</commit_message>
<xml_diff>
--- a/ProyectoMaterias/Formación/Materiales lista precioimport vs precio.xlsx
+++ b/ProyectoMaterias/Formación/Materiales lista precioimport vs precio.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
   <si>
     <t>Material</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Heladera</t>
   </si>
   <si>
-    <t>Utensilios de cocina (platos, cubiertos, escurridor)</t>
-  </si>
-  <si>
     <t>Aire acondicionado</t>
   </si>
   <si>
@@ -203,6 +200,33 @@
   </si>
   <si>
     <t>Precio Total</t>
+  </si>
+  <si>
+    <t>Utensilios de cocina</t>
+  </si>
+  <si>
+    <t>Cubiertos</t>
+  </si>
+  <si>
+    <t>Pack de 12 cuchillos, tenedores y cucharas</t>
+  </si>
+  <si>
+    <t>Platos</t>
+  </si>
+  <si>
+    <t>Escurridor</t>
+  </si>
+  <si>
+    <t>Vasos</t>
+  </si>
+  <si>
+    <t>2 packs de 4 cámaras</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>2 Pack de 1 mesa y 4 sillas</t>
   </si>
 </sst>
 </file>
@@ -270,7 +294,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -358,12 +382,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -428,6 +502,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -744,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,6 +852,8 @@
     <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="47" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -768,16 +864,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -786,7 +882,7 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2">
         <v>7</v>
@@ -805,7 +901,7 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
         <v>20</v>
@@ -824,7 +920,7 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>10</v>
@@ -833,7 +929,7 @@
         <v>400</v>
       </c>
       <c r="F4" s="14">
-        <f t="shared" ref="F4:F13" si="0">E4*D4</f>
+        <f t="shared" ref="F4:F15" si="0">E4*D4</f>
         <v>4000</v>
       </c>
     </row>
@@ -843,7 +939,7 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -862,7 +958,7 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -877,11 +973,13 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -900,7 +998,7 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -919,7 +1017,7 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
@@ -932,38 +1030,44 @@
         <v>7968</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3">
-        <v>3</v>
-      </c>
-      <c r="E10" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="E10" s="29">
+        <v>7200</v>
+      </c>
       <c r="F10" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>E10*D10</f>
+        <v>14400</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="18">
+        <v>6592</v>
+      </c>
       <c r="F11" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>E11*D11</f>
+        <v>13184</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -972,32 +1076,30 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="3">
-        <v>7</v>
-      </c>
-      <c r="E12" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="E12" s="18">
+        <v>4448</v>
+      </c>
       <c r="F12" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>E12*D12</f>
+        <v>13344</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="3">
-        <v>3</v>
-      </c>
-      <c r="E13" s="20"/>
+      <c r="A13" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
       <c r="F13" s="14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(F2:F12)</f>
+        <v>111136</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1006,388 +1108,483 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="21"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="27"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>31</v>
+      <c r="A15" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="3">
-        <v>8</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="D16" s="28">
+        <v>24</v>
+      </c>
+      <c r="E16" s="18">
+        <v>20</v>
+      </c>
+      <c r="F16" s="25">
+        <f>E16*D16</f>
+        <v>480</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="3">
-        <v>12</v>
-      </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="D17" s="28">
+        <v>24</v>
+      </c>
+      <c r="E17" s="29">
+        <v>15</v>
+      </c>
+      <c r="F17" s="25">
+        <f>E17*D17</f>
+        <v>360</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="3">
+        <v>50</v>
+      </c>
+      <c r="D18" s="28">
         <v>1</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E18" s="18">
+        <v>1290</v>
+      </c>
+      <c r="F18" s="25">
+        <f>E18*D18</f>
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="3"/>
+        <v>59</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="C19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="E19" s="18">
+        <v>390</v>
+      </c>
+      <c r="F19" s="25">
+        <f>E19*D19</f>
+        <v>780</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="3">
-        <v>2</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" s="3">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="6"/>
+      <c r="A25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D28" s="3">
+        <v>4</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D29" s="3">
+        <v>3</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D30" s="3">
+        <v>3</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="4"/>
+    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>4</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E35" s="20"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" s="23" t="s">
-        <v>7</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E36" s="20"/>
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>10</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E37" s="20"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>10</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E38" s="20"/>
       <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E39" s="23" t="s">
-        <v>15</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E39" s="20"/>
       <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="20"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" s="23" t="s">
+      <c r="C46" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F46" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E40" r:id="rId1" display="UYU 1249 Link"/>
-    <hyperlink ref="E35" r:id="rId2"/>
-    <hyperlink ref="E39" r:id="rId3"/>
-    <hyperlink ref="E36" r:id="rId4"/>
+    <hyperlink ref="E46" r:id="rId1" display="UYU 1249 Link"/>
+    <hyperlink ref="E41" r:id="rId2"/>
+    <hyperlink ref="E45" r:id="rId3"/>
+    <hyperlink ref="E42" r:id="rId4"/>
     <hyperlink ref="E2" r:id="rId5" display="https://articulo.mercadolibre.com.uy/MLU-445279074-escritorio-mesa-de-pc-con-cajon-oficina-mueble-lcm-_JM"/>
     <hyperlink ref="E5" r:id="rId6" display="https://articulo.mercadolibre.com.uy/MLU-442899266-mueble-cocina-multiuso-armari-living-oficina-2401-_JM"/>
     <hyperlink ref="E3" r:id="rId7" display="https://articulo.mercadolibre.com.uy/MLU-443808655-silla-fija-eco-de-escritorio-oficina-hogar-apilable-armada-_JM"/>
@@ -1396,8 +1593,15 @@
     <hyperlink ref="E7" r:id="rId10" display="https://articulo.mercadolibre.com.uy/MLU-444478827-juego-de-mesa-y-sillas-comedor-o-cocina-varios-modelos-gh-_JM"/>
     <hyperlink ref="E8" r:id="rId11" display="https://articulo.mercadolibre.com.uy/MLU-447144410-microondas-panavox-express-20-digital-el-mejor-respaldo-_JM"/>
     <hyperlink ref="E9" r:id="rId12" display="https://articulo.mercadolibre.com.uy/MLU-452575969-refrigerador-heladera-electrolux-re31-de-240l-oferta-loi-_JM"/>
+    <hyperlink ref="E19" r:id="rId13" display="https://articulo.mercadolibre.com.uy/MLU-453411200-tenedor-mesa-x-12-acero-inoxidable-cuchillo-cuchara-rsi12-_JM"/>
+    <hyperlink ref="E18" r:id="rId14" location="D[S:ADV,L:VQCATCORE_LST,V:2,I:MTU0MDM4OTA0MTc1N3xlLTAwMDFiYWJjfHBsYXktYWtrYS5hY3Rvci5wcm9taXNlcy1kaXNwYXRjaGVyLTQzOXwxMjkzNjA4Mjc1MDg3MzkxNTQ" display="https://articulo.mercadolibre.com.uy/MLU-456463992-escurridor-de-plato-de-dos-niveles-con-bandeja-super-oferta-_JM - D[S:ADV,L:VQCATCORE_LST,V:2,I:MTU0MDM4OTA0MTc1N3xlLTAwMDFiYWJjfHBsYXktYWtrYS5hY3Rvci5wcm9taXNlcy1kaXNwYXRjaGVyLTQzOXwxMjkzNjA4Mjc1MDg3MzkxNTQ"/>
+    <hyperlink ref="E16" r:id="rId15" display="https://articulo.mercadolibre.com.uy/MLU-453665825-plato-melamina-llano-blanco-de-23cm-cu-el-regalon-_JM"/>
+    <hyperlink ref="E17" r:id="rId16" display="https://articulo.mercadolibre.com.uy/MLU-445344546-vaso-vidrio-de-refresco-350-ml-linea-cylinder-nf-_JM"/>
+    <hyperlink ref="E10" r:id="rId17" display="https://articulo.mercadolibre.com.uy/MLU-451528205-aire-acondicionado-corner-celling-12000btu-_JM"/>
+    <hyperlink ref="E11" r:id="rId18" display="https://articulo.mercadolibre.com.uy/MLU-452936573-kit-vigilancia-8-canales-4-cam-hd-todo-incluido--_JM"/>
+    <hyperlink ref="E12" r:id="rId19" display="https://articulo.mercadolibre.com.uy/MLU-449952276-telefono-inal-2-bases-panasonic-captor-y-contest-yanett-_JM"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Materiales lista precioimport vs precio.xlsx - modificado
</commit_message>
<xml_diff>
--- a/ProyectoMaterias/Formación/Materiales lista precioimport vs precio.xlsx
+++ b/ProyectoMaterias/Formación/Materiales lista precioimport vs precio.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
   <si>
     <t>Material</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Herramientas de trabajo:</t>
   </si>
   <si>
-    <t>Computadoras</t>
-  </si>
-  <si>
     <t>Torres</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>Costo Variable</t>
   </si>
   <si>
-    <t>Costos:</t>
-  </si>
-  <si>
     <t>Precio Unitario</t>
   </si>
   <si>
@@ -227,6 +221,18 @@
   </si>
   <si>
     <t>2 Pack de 1 mesa y 4 sillas</t>
+  </si>
+  <si>
+    <t>Costos Fijos:</t>
+  </si>
+  <si>
+    <t>Costos Variables:</t>
+  </si>
+  <si>
+    <t>-------------------------</t>
+  </si>
+  <si>
+    <t>Comintores</t>
   </si>
 </sst>
 </file>
@@ -437,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -448,11 +454,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -471,23 +475,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -509,11 +502,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -522,6 +517,50 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -838,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:B16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,30 +889,33 @@
     <col min="2" max="2" width="39.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="35" customWidth="1"/>
+    <col min="8" max="8" width="35" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
     <col min="12" max="12" width="47" customWidth="1"/>
     <col min="14" max="14" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>57</v>
+      <c r="D1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -882,15 +924,15 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="2">
         <v>7</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="28">
         <v>985</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="32">
         <f>E2*D2</f>
         <v>6895</v>
       </c>
@@ -901,15 +943,15 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="3">
         <v>20</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="29">
         <v>599</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="33">
         <f>E3*D3</f>
         <v>11980</v>
       </c>
@@ -920,15 +962,15 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="3">
         <v>10</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="12">
         <v>400</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="33">
         <f t="shared" ref="F4:F15" si="0">E4*D4</f>
         <v>4000</v>
       </c>
@@ -939,15 +981,15 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="30">
         <v>1390</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="33">
         <f t="shared" si="0"/>
         <v>2780</v>
       </c>
@@ -958,36 +1000,36 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="12">
         <v>3790</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="33">
         <f t="shared" si="0"/>
         <v>3790</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="12">
         <v>14990</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="33">
         <f t="shared" si="0"/>
         <v>29980</v>
       </c>
@@ -998,15 +1040,15 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="12">
         <v>2815</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="33">
         <f t="shared" si="0"/>
         <v>2815</v>
       </c>
@@ -1017,15 +1059,15 @@
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="12">
         <v>7968</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="33">
         <f t="shared" si="0"/>
         <v>7968</v>
       </c>
@@ -1036,15 +1078,15 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="3">
         <v>2</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="31">
         <v>7200</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="33">
         <f>E10*D10</f>
         <v>14400</v>
       </c>
@@ -1054,18 +1096,18 @@
         <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="12">
         <v>6592</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="33">
         <f>E11*D11</f>
         <v>13184</v>
       </c>
@@ -1076,515 +1118,651 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="3">
         <v>3</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="12">
         <v>4448</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="33">
         <f>E12*D12</f>
         <v>13344</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="14">
+      <c r="A13" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="33">
         <f>SUM(F2:F12)</f>
         <v>111136</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="27"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="5"/>
+      <c r="A15" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="28">
+        <v>49</v>
+      </c>
+      <c r="D16" s="20">
         <v>24</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="12">
         <v>20</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="18">
         <f>E16*D16</f>
         <v>480</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="28">
+        <v>49</v>
+      </c>
+      <c r="D17" s="20">
         <v>24</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="31">
         <v>15</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="18">
         <f>E17*D17</f>
         <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="28">
+        <v>49</v>
+      </c>
+      <c r="D18" s="20">
         <v>1</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="12">
         <v>1290</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="18">
         <f>E18*D18</f>
         <v>1290</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="12">
         <v>390</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="18">
         <f>E19*D19</f>
         <v>780</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="6"/>
+      <c r="A20" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="36">
+        <f>SUM(F16:F19)</f>
+        <v>2910</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="3">
-        <v>8</v>
-      </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="3">
-        <v>12</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="E23" s="12">
+        <v>3190</v>
+      </c>
+      <c r="F23" s="36">
+        <f>E23*D23</f>
+        <v>25520</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="3">
-        <v>1</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="E24" s="12">
+        <v>10858</v>
+      </c>
+      <c r="F24" s="36">
+        <f t="shared" ref="F24:F32" si="1">E24*D24</f>
+        <v>130296</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="3">
-        <v>1</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="E25" s="12">
+        <v>2688</v>
+      </c>
+      <c r="F25" s="36">
+        <f t="shared" si="1"/>
+        <v>5376</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="3">
-        <v>2</v>
-      </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="21">
+        <v>6190</v>
+      </c>
+      <c r="F26" s="36">
+        <f t="shared" si="1"/>
+        <v>6190</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="3">
         <v>2</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="41">
+        <v>32000</v>
+      </c>
+      <c r="F27" s="36">
+        <f t="shared" si="1"/>
+        <v>64000</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="3">
-        <v>4</v>
-      </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="12">
+        <v>1216</v>
+      </c>
+      <c r="F28" s="36">
+        <f t="shared" si="1"/>
+        <v>2432</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" s="3">
-        <v>3</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="3">
         <v>3</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="6"/>
+      <c r="E30" s="12">
+        <v>3840</v>
+      </c>
+      <c r="F30" s="36">
+        <f t="shared" si="1"/>
+        <v>11520</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="A32" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="22"/>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="F32" s="36">
+        <f>SUM(F23:F31)</f>
+        <v>245334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="37"/>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="37"/>
+    </row>
+    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="20"/>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="M39" s="26"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M42" s="26"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="8" t="s">
+      <c r="D43" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="M43" s="26"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="20"/>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="D44" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="M44" s="26"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="8" t="s">
+      <c r="C45" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="M45" s="26"/>
+    </row>
+    <row r="46" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="M46" s="26"/>
+    </row>
+    <row r="47" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="M47" s="26"/>
+    </row>
+    <row r="48" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="M48" s="26"/>
+    </row>
+    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="M49" s="26"/>
+    </row>
+    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="4"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F46" s="4"/>
+      <c r="D51" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="F51" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="39"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A32:E32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E46" r:id="rId1" display="UYU 1249 Link"/>
-    <hyperlink ref="E41" r:id="rId2"/>
-    <hyperlink ref="E45" r:id="rId3"/>
-    <hyperlink ref="E42" r:id="rId4"/>
+    <hyperlink ref="E50" r:id="rId1" display="UYU 1249 Link"/>
+    <hyperlink ref="E45" r:id="rId2"/>
+    <hyperlink ref="E49" r:id="rId3"/>
+    <hyperlink ref="E46" r:id="rId4"/>
     <hyperlink ref="E2" r:id="rId5" display="https://articulo.mercadolibre.com.uy/MLU-445279074-escritorio-mesa-de-pc-con-cajon-oficina-mueble-lcm-_JM"/>
     <hyperlink ref="E5" r:id="rId6" display="https://articulo.mercadolibre.com.uy/MLU-442899266-mueble-cocina-multiuso-armari-living-oficina-2401-_JM"/>
     <hyperlink ref="E3" r:id="rId7" display="https://articulo.mercadolibre.com.uy/MLU-443808655-silla-fija-eco-de-escritorio-oficina-hogar-apilable-armada-_JM"/>
@@ -1600,8 +1778,15 @@
     <hyperlink ref="E10" r:id="rId17" display="https://articulo.mercadolibre.com.uy/MLU-451528205-aire-acondicionado-corner-celling-12000btu-_JM"/>
     <hyperlink ref="E11" r:id="rId18" display="https://articulo.mercadolibre.com.uy/MLU-452936573-kit-vigilancia-8-canales-4-cam-hd-todo-incluido--_JM"/>
     <hyperlink ref="E12" r:id="rId19" display="https://articulo.mercadolibre.com.uy/MLU-449952276-telefono-inal-2-bases-panasonic-captor-y-contest-yanett-_JM"/>
+    <hyperlink ref="E23" r:id="rId20" display="http://www.carlosgutierrez.com.uy/show.asp?articulo=6733"/>
+    <hyperlink ref="E24" r:id="rId21" display="http://www.carlosgutierrez.com.uy/show.asp?articulo=7236"/>
+    <hyperlink ref="E25" r:id="rId22" display="https://articulo.mercadolibre.com.uy/MLU-444624855-impresora-multifuncion-epson-wifi-xp241-tintas-originales-_JM"/>
+    <hyperlink ref="E26" r:id="rId23" display="http://www.carlosgutierrez.com.uy/show.asp?articulo=6901"/>
+    <hyperlink ref="E27" r:id="rId24" display="https://articulo.mercadolibre.com.uy/MLU-444511947-racks-servidores-42u-gabinetes-computacion-ventilados-server-_JM"/>
+    <hyperlink ref="E28" r:id="rId25" display="https://articulo.mercadolibre.com.uy/MLU-449515129-patchera-24-puertos-cat-6e-para-rack-_JM"/>
+    <hyperlink ref="E30" r:id="rId26" location="D[S:ADV,L:VQCATCORE_LST,V:3,I:MTU0MDM5MzU0NTM1N3xlLTAwMDE5YWI5fHBsYXktYWtrYS5hY3Rvci5wcm9taXNlcy1kaXNwYXRjaGVyLTIwOXwyMDQxNzY1NDM3NjIwMjU4MTYz," display="https://articulo.mercadolibre.com.uy/MLU-451119915-access-point-tp-link-eap220-600mbps-montaje-en-techopared-_JM - D[S:ADV,L:VQCATCORE_LST,V:3,I:MTU0MDM5MzU0NTM1N3xlLTAwMDE5YWI5fHBsYXktYWtrYS5hY3Rvci5wcm9taXNlcy1kaXNwYXRjaGVyLTIwOXwyMDQxNzY1NDM3NjIwMjU4MTYz,"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>